<commit_message>
make it possible to exclude hubs
</commit_message>
<xml_diff>
--- a/EMPIRE-OW/Data handler/offshore_wind/Generator.xlsx
+++ b/EMPIRE-OW/Data handler/offshore_wind/Generator.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ivergjorvad/Desktop/prosjektoppgave/IverEMPIRE-base/Data handler/offshore_wind/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ivergjorvad/Desktop/prosjektoppgave/EMPIRE-OW/Data handler/offshore_wind/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D51351A-7AE7-3947-AE30-EEA2020DDD77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F2AE954-A3D3-B94E-BCBB-DCF09C692FD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="25800" windowHeight="15800" tabRatio="788" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>

</xml_diff>